<commit_message>
image test and labels
</commit_message>
<xml_diff>
--- a/data/swim_locations.xlsx
+++ b/data/swim_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\langt\Documents\GitHub\swim_nl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0740665A-254D-4975-89A5-84B4B2B5D50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6922F91-9C2A-4247-98CA-890600B7179C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{2B70663B-0FB2-4909-BB90-064EC3C674D3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -46,40 +46,70 @@
     <t>Contributor</t>
   </si>
   <si>
-    <t>Sloterplas</t>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>Sloterplas (North pier)</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>Sloterplas (North beach)</t>
+  </si>
+  <si>
+    <t>Official</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Diemerpark strand</t>
+  </si>
+  <si>
+    <t>Photos</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c1/Rlogo.png/274px-Rlogo.png</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>No photo yet</t>
+  </si>
+  <si>
+    <t>Official swim spot</t>
+  </si>
+  <si>
+    <t>Not official swim spot</t>
   </si>
   <si>
     <t>Ladder entry</t>
   </si>
   <si>
-    <t>Ladder exit</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Depth at entry</t>
-  </si>
-  <si>
-    <t>2m</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lng</t>
+    <t>Beach entry</t>
+  </si>
+  <si>
+    <t>Too shallow for proper swimming</t>
+  </si>
+  <si>
+    <t>Popular spot for swimmers</t>
+  </si>
+  <si>
+    <t>Popular for families</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,9 +139,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,73 +455,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C6819C-BBBA-4479-8140-6127426582A1}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
     <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" customWidth="1"/>
     <col min="6" max="6" width="16.08984375" customWidth="1"/>
-    <col min="7" max="8" width="13.7265625" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" customWidth="1"/>
+    <col min="8" max="9" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>52.370597600000004</v>
+      </c>
+      <c r="I2">
+        <v>4.8209964999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>52.371551400000001</v>
+      </c>
+      <c r="I3">
+        <v>4.8225343000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1">
-        <v>52.370086499999999</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4.8200564000000004</v>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>52.354283799999997</v>
+      </c>
+      <c r="I4">
+        <v>4.9843270999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>